<commit_message>
Configuración maneja si api_apagada
</commit_message>
<xml_diff>
--- a/iteracionesTest.xlsx
+++ b/iteracionesTest.xlsx
@@ -513,7 +513,11 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>

</xml_diff>

<commit_message>
Full results reporting ready Ok!
</commit_message>
<xml_diff>
--- a/iteracionesTest.xlsx
+++ b/iteracionesTest.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>URL4</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>URL0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -491,11 +496,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEi0TQ389Qscw,Take=1,Shot=3quarters-mediumshot,Style=dibujo.png</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEi0TQ389Qscw,Take=2,Shot=front-mediumshot2,Style=art nouveau.png</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEi0TQ389Qscw,Take=3,Shot=3quarters-mediumshot6,Style=painting.png</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEi0TQ389Qscw,Take=0,Shot=front-mediumshot,Style=anime.png</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -515,13 +541,30 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEmlDyj9hAsCw,Take=1,Shot=3quarters-mediumshot2,Style=dibujo.png</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEmlDyj9hAsCw,Take=2,Shot=front-mediumshot5,Style=picture.png</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEmlDyj9hAsCw,Take=3,Shot=3quarters-mediumshot,Style=art nouveau.png</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEmlDyj9hAsCw,Take=0,Shot=3quarters-mediumshot,Style=watercolor.png</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -539,11 +582,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEplXHfRlPCaQ,Take=1,Shot=front-mediumshot7,Style=impresionist.png</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEplXHfRlPCaQ,Take=2,Shot=front-mediumshot2,Style=comic.png</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEplXHfRlPCaQ,Take=3,Shot=3quarters-mediumshot5,Style=picture.png</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEplXHfRlPCaQ,Take=0,Shot=front-mediumshot10,Style=impresionist.png</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -561,11 +625,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEpRmJSwSA4oA,Take=1,Shot=profile-mediumshot,Style=painting.png</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEpRmJSwSA4oA,Take=2,Shot=front-mediumshot4,Style=dibujo.png</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEpRmJSwSA4oA,Take=3,Shot=front-mediumshot,Style=watercolor.png</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEpRmJSwSA4oA,Take=0,Shot=front-mediumshotdown1,Style=pop-art.png</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -583,11 +668,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEqEv9D5aV9UA,Take=1,Shot=front-mediumshotdown1,Style=watercolor.png</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEqEv9D5aV9UA,Take=2,Shot=front-mediumshot8,Style=pop-art.png</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEqEv9D5aV9UA,Take=3,Shot=3quarters-mediumshotdown,Style=picture.png</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEqEv9D5aV9UA,Take=0,Shot=3quarters-mediumshot5,Style=japanese-style.png</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -605,11 +711,20 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEwDPgclRcUPg,Take=0,Shot=front-mediumshot7,Style=art nouveau.png</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -627,11 +742,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEWTnGx_ue9vw,Take=1,Shot=front-mediumshot7,Style=pop-art.png</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEWTnGx_ue9vw,Take=2,Shot=3quarters-mediumshot5,Style=watercolor.png</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEWTnGx_ue9vw,Take=3,Shot=front-mediumshot3,Style=watercolor.png</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEWTnGx_ue9vw,Take=0,Shot=3quarters-mediumshotdown,Style=watercolor.png</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -649,11 +785,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEXgxCdjGrCcw,Take=1,Shot=front-mediumshot,Style=anime.png</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEXgxCdjGrCcw,Take=2,Shot=front-mediumshot9,Style=watercolor.png</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEXgxCdjGrCcw,Take=3,Shot=front-mediumshot5,Style=japanese-animation.png</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEXgxCdjGrCcw,Take=0,Shot=front-mediumshot,Style=japanese-style.png</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -671,11 +828,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEZs8qD93Q7IQ,Take=1,Shot=3quarters-mediumshotdown,Style=watercolor.png</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEZs8qD93Q7IQ,Take=2,Shot=front-mediumshot7,Style=comic.png</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEZs8qD93Q7IQ,Take=3,Shot=3quarters-mediumshotdown,Style=watercolor.png</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQEZs8qD93Q7IQ,Take=0,Shot=front-americanshot1,Style=pop-art.png</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -698,6 +876,7 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -715,11 +894,28 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFACwauUG_weQ,Take=1,Shot=3quarters-mediumshotdown,Style=dibujo.png</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFACwauUG_weQ,Take=2,Shot=front-mediumshot3,Style=impresionist.png</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFACwauUG_weQ,Take=0,Shot=3quarters-mediumshot,Style=impresionist.png</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -737,11 +933,24 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFl26ghRa-DNA,Take=1,Shot=3quarters-mediumshot3,Style=manga.png</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFl26ghRa-DNA,Take=0,Shot=front-mediumshot7,Style=manga.png</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -759,11 +968,16 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -781,11 +995,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFosZAfNf4HQA,Take=1,Shot=front-mediumshotdown,Style=lineart.png</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFosZAfNf4HQA,Take=2,Shot=3quarters-mediumshotdown,Style=impresionist.png</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFosZAfNf4HQA,Take=3,Shot=front-mediumshot9,Style=pop-art.png</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFosZAfNf4HQA,Take=0,Shot=front-mediumshot10,Style=japanese-animation.png</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -803,11 +1038,16 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Unable to detect a face in the image. Please upload a different photo with a clear face.'</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -825,11 +1065,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFttq8Hu6iXjQ,Take=1,Shot=front-americanshot,Style=art nouveau.png</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFttq8Hu6iXjQ,Take=2,Shot=front-mediumshot5,Style=watercolor.png</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFttq8Hu6iXjQ,Take=3,Shot=front-mediumshotdown1,Style=anime.png</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFttq8Hu6iXjQ,Take=0,Shot=front-mediumdownshot,Style=japanese-animation.png</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -847,11 +1108,24 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFUo0Ia6oDqqQ,Take=1,Shot=3quarters-mediumshotdown,Style=art nouveau.png</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFUo0Ia6oDqqQ,Take=0,Shot=front-mediumshot6,Style=impresionist.png</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -869,11 +1143,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFyc6p5eQ-ZEQ,Take=1,Shot=3quarters-mediumshot1,Style=anime.png</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFyc6p5eQ-ZEQ,Take=2,Shot=front-mediumshot4,Style=picture.png</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFyc6p5eQ-ZEQ,Take=3,Shot=3quarters-mediumshotdown,Style=watercolor.png</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQFyc6p5eQ-ZEQ,Take=0,Shot=front-mediumshot9,Style=painting.png</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -891,11 +1186,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQG_bg8qzvb2uQ,Take=1,Shot=front-mediumshot1,Style=japanese-style.png</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQG_bg8qzvb2uQ,Take=2,Shot=front-mediumshot4,Style=manga.png</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQG_bg8qzvb2uQ,Take=3,Shot=3quarters-mediumshot1,Style=art nouveau.png</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQG_bg8qzvb2uQ,Take=0,Shot=3quarters-mediumshot4,Style=impresionist.png</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -913,11 +1229,16 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -935,11 +1256,20 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGC2PW9R5LQcw,Take=0,Shot=3quarters-mediumshotdown,Style=watercolor.png</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -957,11 +1287,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGD50pmZoRmOg,Take=1,Shot=front-mediumshot,Style=art nouveau.png</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGD50pmZoRmOg,Take=2,Shot=3quarters-mediumshot,Style=picture.png</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGD50pmZoRmOg,Take=3,Shot=front-mediumshot5,Style=comic.png</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGD50pmZoRmOg,Take=0,Shot=front-americanshot,Style=japanese-animation.png</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -979,11 +1330,24 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGfpL3OdJ-ENg,Take=1,Shot=profile-mediumshot,Style=comic-book.png</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGfpL3OdJ-ENg,Take=0,Shot=3quarters-mediumshotdown,Style=impresionist.png</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1006,6 +1370,7 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1023,11 +1388,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGjVV-W59A6Bw,Take=1,Shot=3quarters-mediumshot2,Style=art nouveau.png</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGjVV-W59A6Bw,Take=2,Shot=front-mediumshot,Style=art nouveau.png</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGjVV-W59A6Bw,Take=3,Shot=3quarters-mediumshot5,Style=dibujo.png</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGjVV-W59A6Bw,Take=0,Shot=front-mediumshot10,Style=manga.png</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1045,11 +1431,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGlpQeX43jVTw,Take=1,Shot=front-mediumshot2,Style=comic-book.png</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGlpQeX43jVTw,Take=2,Shot=3quarters-mediumshot,Style=impresionist.png</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGlpQeX43jVTw,Take=3,Shot=front-mediumshot9,Style=comic.png</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQGlpQeX43jVTw,Take=0,Shot=front-americanshot,Style=comic-book.png</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1067,11 +1474,16 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Unable to detect a face in the image. Please upload a different photo with a clear face.'</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1089,11 +1501,16 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Unable to detect a face in the image. Please upload a different photo with a clear face.'</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1116,6 +1533,7 @@
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1133,11 +1551,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQH2s4692Es2ng,Take=1,Shot=front-mediumshot10,Style=watercolor.png</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQH2s4692Es2ng,Take=2,Shot=front-mediumshotdown2,Style=manga.png</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQH2s4692Es2ng,Take=3,Shot=3quarters-mediumshot1,Style=watercolor.png</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQH2s4692Es2ng,Take=0,Shot=front-mediumshot6,Style=painting.png</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1155,11 +1594,16 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Unable to detect a face in the image. Please upload a different photo with a clear face.'</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1177,11 +1621,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQH7R3JcHaTdMw,Take=1,Shot=front-mediumshotdown1,Style=japanese-style.png</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQH7R3JcHaTdMw,Take=2,Shot=front-mediumshot7,Style=comic.png</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQH7R3JcHaTdMw,Take=3,Shot=3quarters-mediumshotdown,Style=anime.png</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQH7R3JcHaTdMw,Take=0,Shot=front-mediumshot10,Style=art nouveau.png</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1199,11 +1664,32 @@
           <t>Success</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Image processed</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQHaA_NSAx1ZAQ,Take=1,Shot=front-mediumshot8,Style=comic.png</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQHaA_NSAx1ZAQ,Take=2,Shot=front-americanshot1,Style=manga.png</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQHaA_NSAx1ZAQ,Take=3,Shot=3quarters-mediumshotdown,Style=watercolor.png</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>https://euroglitter.com/results/iteracionesTest/C4D03AQHaA_NSAx1ZAQ,Take=0,Shot=front-mediumshot8,Style=impresionist.png</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>